<commit_message>
reject demands with ammouns less than 1 pallet
</commit_message>
<xml_diff>
--- a/Model/Database Input/Error_Demand.xlsx
+++ b/Model/Database Input/Error_Demand.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G144"/>
+  <dimension ref="A1:G147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Order Number</t>
+          <t>Work Order</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -494,7 +494,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -525,7 +525,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -556,7 +556,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -587,7 +587,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -620,7 +620,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -653,7 +653,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -686,7 +686,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -696,12 +696,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>50006126</t>
+          <t>50006835</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>WO21008109</t>
+          <t>WO21009387</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -711,15 +711,15 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>30002220</t>
+          <t>30003904</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>300</v>
+        <v>2640</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -729,12 +729,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>50006835</t>
+          <t>50006838</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>WO21009387</t>
+          <t>WO21009392</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -744,15 +744,15 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>30003904</t>
+          <t>30003943</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>2640</v>
+        <v>1062</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -762,12 +762,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>50008061</t>
+          <t>50000550</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>WO21005721</t>
+          <t>WO21008593</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -777,15 +777,15 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>30002080</t>
+          <t>30002277</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>150</v>
+        <v>29837</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -795,12 +795,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>50006838</t>
+          <t>50008297</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>WO21009392</t>
+          <t>WO21008607</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -810,15 +810,15 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>30003943</t>
+          <t>30002011</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>1062</v>
+        <v>1800</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G12" t="n">
@@ -828,12 +828,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>50000550</t>
+          <t>50005989</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>WO21008593</t>
+          <t>WO21008628</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -843,15 +843,15 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>30002277</t>
+          <t>30002078</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>29837</v>
+        <v>7000</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G13" t="n">
@@ -861,12 +861,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>50008297</t>
+          <t>50006828</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>WO21008607</t>
+          <t>WO21009273</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -876,15 +876,15 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>30002011</t>
+          <t>30003941</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>1800</v>
+        <v>1100</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G14" t="n">
@@ -894,12 +894,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>50005989</t>
+          <t>50006834</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>WO21008628</t>
+          <t>WO21009378</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -909,15 +909,15 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>30002078</t>
+          <t>30003911</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>7000</v>
+        <v>560</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G15" t="n">
@@ -927,12 +927,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>50006828</t>
+          <t>50008297</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>WO21009273</t>
+          <t>WO21009910</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -942,15 +942,15 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>30003941</t>
+          <t>30002011</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>1100</v>
+        <v>1200</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G16" t="n">
@@ -960,12 +960,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>50006834</t>
+          <t>50006126</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>WO21009378</t>
+          <t>WO21010192</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -975,15 +975,15 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>30003911</t>
+          <t>30002220</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>3430</v>
+        <v>6520</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G17" t="n">
@@ -993,12 +993,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>50006831</t>
+          <t>50006677</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>WO21009374</t>
+          <t>WO21004530</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1008,15 +1008,15 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>30003905</t>
+          <t>30002053</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>420</v>
+        <v>11302</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G18" t="n">
@@ -1026,12 +1026,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>50008297</t>
+          <t>50008690</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>WO21009910</t>
+          <t>WO21005209</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1041,15 +1041,15 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>30002011</t>
+          <t>30004029</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>1200</v>
+        <v>675</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G19" t="n">
@@ -1059,12 +1059,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>50006126</t>
+          <t>50008689</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>WO21010192</t>
+          <t>WO21005210</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1074,15 +1074,15 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>30002220</t>
+          <t>30004029</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>19720</v>
+        <v>675</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -1092,12 +1092,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>50006677</t>
+          <t>50008854</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>WO21004530</t>
+          <t>WO21010078</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1107,15 +1107,15 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>30002053</t>
+          <t>30004094</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>11302</v>
+        <v>5120</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G21" t="n">
@@ -1125,12 +1125,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>50008690</t>
+          <t>50008846</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>WO21005209</t>
+          <t>WO21010084</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1140,15 +1140,15 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>30004029</t>
+          <t>30004096</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>675</v>
+        <v>5120</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G22" t="n">
@@ -1158,12 +1158,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>50008689</t>
+          <t>50000360</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>WO21005210</t>
+          <t>WO21010071</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1173,15 +1173,15 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>30004029</t>
+          <t>30001908</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>675</v>
+        <v>32730</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -1191,12 +1191,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>50008854</t>
+          <t>50006837</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>WO21010078</t>
+          <t>WO21016504</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1206,15 +1206,15 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>30004094</t>
+          <t>30003904</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>5120</v>
+        <v>52500</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -1224,12 +1224,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>50008846</t>
+          <t>50006830</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>WO21010084</t>
+          <t>WO21016490</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1239,15 +1239,15 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>30004096</t>
+          <t>30003941</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>5120</v>
+        <v>47250</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G25" t="n">
@@ -1257,12 +1257,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>50000360</t>
+          <t>50008681</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>WO21010071</t>
+          <t>WO21012827</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1272,15 +1272,15 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>30001908</t>
+          <t>30002524</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>32730</v>
+        <v>142</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G26" t="n">
@@ -1290,12 +1290,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>50006837</t>
+          <t>50008848</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>WO21016504</t>
+          <t>WO21014432</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1305,15 +1305,15 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>30003904</t>
+          <t>30004095</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>52500</v>
+        <v>5120</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G27" t="n">
@@ -1323,12 +1323,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>50006830</t>
+          <t>50000483</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>WO21016490</t>
+          <t>WO21014440</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1338,15 +1338,15 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>30003941</t>
+          <t>30002094</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>47250</v>
+        <v>80640</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -1356,12 +1356,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>50008681</t>
+          <t>50000435</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>WO21012827</t>
+          <t>WO21014776</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1371,15 +1371,15 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>30002524</t>
+          <t>30001905</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>142</v>
+        <v>9999</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G29" t="n">
@@ -1389,12 +1389,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>50008848</t>
+          <t>50000605</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>WO21014432</t>
+          <t>WO21017288</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1404,15 +1404,15 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>30004095</t>
+          <t>30002113</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>5120</v>
+        <v>20000</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G30" t="n">
@@ -1422,12 +1422,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>50000483</t>
+          <t>50006831</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>WO21014440</t>
+          <t>WO21016479</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1437,15 +1437,15 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>30002094</t>
+          <t>30003905</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>80640</v>
+        <v>17820</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G31" t="n">
@@ -1455,12 +1455,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>50008215</t>
+          <t>50006833</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>WO21014617</t>
+          <t>WO21016480</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1470,15 +1470,15 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>30000394</t>
+          <t>30003905</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>1056</v>
+        <v>5250</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G32" t="n">
@@ -1488,12 +1488,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>50008215</t>
+          <t>50006840</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>WO21014617</t>
+          <t>WO21016485</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1503,15 +1503,15 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>30002347</t>
+          <t>30003943</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>1056</v>
+        <v>24150</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G33" t="n">
@@ -1521,12 +1521,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>50000435</t>
+          <t>50004282</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>WO21014776</t>
+          <t>WO21015952</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1536,15 +1536,15 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>30001905</t>
+          <t>30002452</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>9999</v>
+        <v>30000</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G34" t="n">
@@ -1554,12 +1554,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>50006831</t>
+          <t>50005987</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>WO21016479</t>
+          <t>WO21014442</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1569,15 +1569,15 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>30003905</t>
+          <t>30000331</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>17820</v>
+        <v>2500</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G35" t="n">
@@ -1587,12 +1587,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>50006833</t>
+          <t>50005987</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>WO21016480</t>
+          <t>WO21014442</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1602,15 +1602,15 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>30003905</t>
+          <t>30002280</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>5250</v>
+        <v>2500</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G36" t="n">
@@ -1620,12 +1620,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>50006840</t>
+          <t>50006569</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>WO21016485</t>
+          <t>WO21017015</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1635,15 +1635,15 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>30003943</t>
+          <t>30002433</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>24150</v>
+        <v>4683</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G37" t="n">
@@ -1653,12 +1653,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>50004282</t>
+          <t>50006838</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>WO21015952</t>
+          <t>WO21016484</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1668,15 +1668,15 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>30002452</t>
+          <t>30003943</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>30000</v>
+        <v>15840</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G38" t="n">
@@ -1686,12 +1686,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>50005987</t>
+          <t>50006677</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>WO21014442</t>
+          <t>WO21017426</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1701,15 +1701,15 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>30000331</t>
+          <t>30002053</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>2500</v>
+        <v>2558</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G39" t="n">
@@ -1719,12 +1719,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>50005987</t>
+          <t>50006678</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>WO21014442</t>
+          <t>WO21017427</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1734,15 +1734,15 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>30002280</t>
+          <t>30002053</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>2500</v>
+        <v>1848</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G40" t="n">
@@ -1752,12 +1752,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>50006079</t>
+          <t>50006665</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>WO21016927</t>
+          <t>WO21017438</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1767,15 +1767,15 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>30002468</t>
+          <t>30002058</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>27000</v>
+        <v>4554</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G41" t="n">
@@ -1785,12 +1785,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>50006569</t>
+          <t>50006666</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>WO21017015</t>
+          <t>WO21017440</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1800,15 +1800,15 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>30002433</t>
+          <t>30002058</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>4683</v>
+        <v>3426</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G42" t="n">
@@ -1818,12 +1818,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>50006838</t>
+          <t>50000483</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>WO21016484</t>
+          <t>WO21017410</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1833,15 +1833,15 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>30003943</t>
+          <t>30002094</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>15840</v>
+        <v>132480</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G43" t="n">
@@ -1851,12 +1851,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>50006834</t>
+          <t>50000609</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>WO21016519</t>
+          <t>WO21017292</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1866,15 +1866,15 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>30003911</t>
+          <t>30002109</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>3630</v>
+        <v>16000</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G44" t="n">
@@ -1884,12 +1884,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>50006828</t>
+          <t>50000611</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>WO21016489</t>
+          <t>WO21017296</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1899,15 +1899,15 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>30003941</t>
+          <t>30002108</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>1100</v>
+        <v>16000</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G45" t="n">
@@ -1917,12 +1917,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>50006865</t>
+          <t>50006834</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>WO21016494</t>
+          <t>WO21016519</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1932,15 +1932,15 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>30003942</t>
+          <t>30003911</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>660</v>
+        <v>3630</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G46" t="n">
@@ -1950,12 +1950,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>50006866</t>
+          <t>50006828</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>WO21016495</t>
+          <t>WO21016489</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1965,15 +1965,15 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>30003942</t>
+          <t>30003941</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>15750</v>
+        <v>1100</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G47" t="n">
@@ -1983,12 +1983,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>50006835</t>
+          <t>50006865</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>WO21016503</t>
+          <t>WO21016494</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1998,15 +1998,15 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>30003904</t>
+          <t>30003942</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>1100</v>
+        <v>660</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G48" t="n">
@@ -2016,12 +2016,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>50006870</t>
+          <t>50006866</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>WO21016513</t>
+          <t>WO21016495</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2031,15 +2031,15 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>30003909</t>
+          <t>30003942</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>2310</v>
+        <v>15750</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G49" t="n">
@@ -2049,12 +2049,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>50006842</t>
+          <t>50006835</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>WO21016522</t>
+          <t>WO21016503</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2064,15 +2064,15 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>30003948</t>
+          <t>30003904</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>15180</v>
+        <v>1100</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G50" t="n">
@@ -2082,12 +2082,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>50000435</t>
+          <t>50006870</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>SON21000804</t>
+          <t>WO21016513</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2097,15 +2097,15 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>30001905</t>
+          <t>30003909</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>9999</v>
+        <v>2310</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G51" t="n">
@@ -2115,12 +2115,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>50000319</t>
+          <t>50006842</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>SON21003483</t>
+          <t>WO21016522</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2130,15 +2130,15 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>30002137</t>
+          <t>30003948</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>2000</v>
+        <v>15180</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G52" t="n">
@@ -2148,12 +2148,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>50000318</t>
+          <t>50000319</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>SON21001159</t>
+          <t>SON21003483</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2163,15 +2163,15 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>30002136</t>
+          <t>30002137</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>960</v>
+        <v>2000</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G53" t="n">
@@ -2181,12 +2181,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>50005993</t>
+          <t>50000338</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>SON21000855</t>
+          <t>SON21003483</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2196,15 +2196,15 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>30002060</t>
+          <t>30002414</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>3000</v>
+        <v>1200</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G54" t="n">
@@ -2214,7 +2214,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>50005991</t>
+          <t>50005993</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2229,7 +2229,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>30002061</t>
+          <t>30002060</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -2237,7 +2237,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G55" t="n">
@@ -2247,12 +2247,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>50005977</t>
+          <t>50005991</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>SON21001057</t>
+          <t>SON21000855</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2262,15 +2262,15 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>30001907</t>
+          <t>30002061</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>3220</v>
+        <v>3000</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G56" t="n">
@@ -2280,12 +2280,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>50000435</t>
+          <t>50005977</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>SON21002081</t>
+          <t>SON21001057</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2295,15 +2295,15 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>30001905</t>
+          <t>30001907</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>624</v>
+        <v>3220</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G57" t="n">
@@ -2313,12 +2313,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>50006126</t>
+          <t>50000435</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>SON21002720</t>
+          <t>SON21002081</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2328,15 +2328,15 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>30002220</t>
+          <t>30001905</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>8000</v>
+        <v>624</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G58" t="n">
@@ -2346,12 +2346,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>50005991</t>
+          <t>50006126</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>SON21006837</t>
+          <t>SON21002720</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2361,15 +2361,15 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>30002061</t>
+          <t>30002220</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>4000</v>
+        <v>8000</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G59" t="n">
@@ -2379,12 +2379,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>50006837</t>
+          <t>50005991</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>SON21002158</t>
+          <t>SON21006837</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2394,15 +2394,15 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>30003904</t>
+          <t>30002061</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>23100</v>
+        <v>4000</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G60" t="n">
@@ -2412,7 +2412,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>50006833</t>
+          <t>50006837</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2427,15 +2427,15 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>30003905</t>
+          <t>30003904</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>2545</v>
+        <v>23100</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G61" t="n">
@@ -2445,12 +2445,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>50000552</t>
+          <t>50006833</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>SON21001472</t>
+          <t>SON21002158</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2460,15 +2460,15 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>30002471</t>
+          <t>30003905</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>2621</v>
+        <v>2545</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G62" t="n">
@@ -2478,12 +2478,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>50006661</t>
+          <t>50000552</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>SON21001488</t>
+          <t>SON21001472</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2493,15 +2493,15 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>30002057</t>
+          <t>30002471</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>512</v>
+        <v>2621</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G63" t="n">
@@ -2511,12 +2511,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>50008144</t>
+          <t>50000314</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>SON21001488</t>
+          <t>SON21002405</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2526,15 +2526,15 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>30003976</t>
+          <t>30002138</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>22</v>
+        <v>5000</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G64" t="n">
@@ -2544,12 +2544,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>50000435</t>
+          <t>50000335</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>SON21000755</t>
+          <t>SON21002405</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2559,15 +2559,15 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>30001905</t>
+          <t>30002141</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>9999</v>
+        <v>3200</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G65" t="n">
@@ -2577,12 +2577,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>50000314</t>
+          <t>50006109</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>SON21002405</t>
+          <t>SON21005127</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2592,15 +2592,15 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>30002138</t>
+          <t>30002241</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>5000</v>
+        <v>30560</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G66" t="n">
@@ -2610,12 +2610,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>50000335</t>
+          <t>50006079</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>SON21002405</t>
+          <t>SON21005127</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2625,15 +2625,15 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>30002141</t>
+          <t>30002468</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>3200</v>
+        <v>26640</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G67" t="n">
@@ -2643,7 +2643,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>50006109</t>
+          <t>50006105</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2658,15 +2658,15 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>30002241</t>
+          <t>30002217</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>30560</v>
+        <v>40000</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G68" t="n">
@@ -2676,12 +2676,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>50006105</t>
+          <t>50006125</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>SON21005127</t>
+          <t>SON21001775</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2691,15 +2691,15 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>30002217</t>
+          <t>30002221</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>40000</v>
+        <v>126000</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G69" t="n">
@@ -2709,7 +2709,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>50006125</t>
+          <t>50006126</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2724,15 +2724,15 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>30002221</t>
+          <t>30002220</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>540</v>
+        <v>6080</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G70" t="n">
@@ -2742,7 +2742,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>50006125</t>
+          <t>50006109</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2757,15 +2757,15 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>30002221</t>
+          <t>30002241</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>126000</v>
+        <v>8192</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G71" t="n">
@@ -2775,7 +2775,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>50006126</t>
+          <t>50006079</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2790,15 +2790,15 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>30002220</t>
+          <t>30002468</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>6080</v>
+        <v>20700</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G72" t="n">
@@ -2808,7 +2808,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>50006109</t>
+          <t>50006114</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2823,15 +2823,15 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>30002241</t>
+          <t>30002226</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>8192</v>
+        <v>15966</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G73" t="n">
@@ -2841,12 +2841,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>50006079</t>
+          <t>50009138</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>SON21001775</t>
+          <t>SON21002984</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2856,15 +2856,15 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>30002468</t>
+          <t>30004104</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>20700</v>
+        <v>576</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G74" t="n">
@@ -2874,12 +2874,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>50006114</t>
+          <t>50009136</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>SON21001775</t>
+          <t>SON21002984</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2889,15 +2889,15 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>30002226</t>
+          <t>30004047</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>15966</v>
+        <v>4764</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G75" t="n">
@@ -2907,12 +2907,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>50009138</t>
+          <t>50006001</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>SON21002984</t>
+          <t>SON21003414</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2922,15 +2922,15 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>30004104</t>
+          <t>30002063</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>576</v>
+        <v>2000</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G76" t="n">
@@ -2940,12 +2940,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>50009136</t>
+          <t>50000314</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>SON21002984</t>
+          <t>SON21003481</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2955,15 +2955,15 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>30004047</t>
+          <t>30002138</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>4764</v>
+        <v>5500</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G77" t="n">
@@ -2973,12 +2973,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>50006677</t>
+          <t>50006126</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>SON21005185</t>
+          <t>SON21003784</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2988,15 +2988,15 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>30002053</t>
+          <t>30002220</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>2558</v>
+        <v>11700</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G78" t="n">
@@ -3006,12 +3006,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>50006678</t>
+          <t>50006125</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>SON21005185</t>
+          <t>SON21003784</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3021,15 +3021,15 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>30002053</t>
+          <t>30002221</t>
         </is>
       </c>
       <c r="E79" t="n">
-        <v>1732</v>
+        <v>10134</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G79" t="n">
@@ -3039,12 +3039,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>50006665</t>
+          <t>50006079</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>SON21005185</t>
+          <t>SON21003784</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3054,15 +3054,15 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>30002058</t>
+          <t>30002468</t>
         </is>
       </c>
       <c r="E80" t="n">
-        <v>4554</v>
+        <v>30204</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G80" t="n">
@@ -3072,12 +3072,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>50006666</t>
+          <t>50008681</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>SON21005185</t>
+          <t>SON21004229</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3087,15 +3087,15 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>30002058</t>
+          <t>30002524</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>3426</v>
+        <v>844</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G81" t="n">
@@ -3105,12 +3105,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>50000314</t>
+          <t>50008300</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>SON21003481</t>
+          <t>SON21006688</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3120,15 +3120,15 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>30002138</t>
+          <t>30002102</t>
         </is>
       </c>
       <c r="E82" t="n">
-        <v>5500</v>
+        <v>13757</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G82" t="n">
@@ -3138,12 +3138,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>50006125</t>
+          <t>50000362</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>SON21003784</t>
+          <t>SON21004762</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3153,15 +3153,15 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>30002221</t>
+          <t>30001917</t>
         </is>
       </c>
       <c r="E83" t="n">
-        <v>10134</v>
+        <v>846</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G83" t="n">
@@ -3171,12 +3171,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>50006079</t>
+          <t>50006840</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>SON21003784</t>
+          <t>SON21004543</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3186,15 +3186,15 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>30002468</t>
+          <t>30003943</t>
         </is>
       </c>
       <c r="E84" t="n">
-        <v>30204</v>
+        <v>2100</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G84" t="n">
@@ -3204,12 +3204,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>50000483</t>
+          <t>50000435</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>SON21005747</t>
+          <t>SON21004833</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3219,15 +3219,15 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>30002094</t>
+          <t>30001905</t>
         </is>
       </c>
       <c r="E85" t="n">
-        <v>132480</v>
+        <v>9999</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G85" t="n">
@@ -3237,12 +3237,12 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>50008681</t>
+          <t>50008215</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>SON21004229</t>
+          <t>SON21005295</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3252,15 +3252,15 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>30002524</t>
+          <t>30000394</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>844</v>
+        <v>1056</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G86" t="n">
@@ -3270,12 +3270,12 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>50008300</t>
+          <t>50008215</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>SON21006688</t>
+          <t>SON21005295</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3285,15 +3285,15 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>30002102</t>
+          <t>30002347</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>13757</v>
+        <v>1056</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G87" t="n">
@@ -3303,12 +3303,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>50000362</t>
+          <t>50000435</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>SON21004762</t>
+          <t>SON21006006</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3318,15 +3318,15 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>30001917</t>
+          <t>30001905</t>
         </is>
       </c>
       <c r="E88" t="n">
-        <v>846</v>
+        <v>19999</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G88" t="n">
@@ -3336,12 +3336,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>50006840</t>
+          <t>50006679</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>SON21004543</t>
+          <t>SON21006253</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3351,15 +3351,15 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>30003943</t>
+          <t>30002056</t>
         </is>
       </c>
       <c r="E89" t="n">
-        <v>2100</v>
+        <v>6369</v>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G89" t="n">
@@ -3369,12 +3369,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>50000435</t>
+          <t>50006680</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>SON21004833</t>
+          <t>SON21006253</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3384,15 +3384,15 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>30001905</t>
+          <t>30002056</t>
         </is>
       </c>
       <c r="E90" t="n">
-        <v>9999</v>
+        <v>2926</v>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G90" t="n">
@@ -3402,12 +3402,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>50000435</t>
+          <t>50006661</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>SON21006006</t>
+          <t>SON21006253</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3417,15 +3417,15 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>30001905</t>
+          <t>30002057</t>
         </is>
       </c>
       <c r="E91" t="n">
-        <v>19999</v>
+        <v>4950</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G91" t="n">
@@ -3435,12 +3435,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>50008760</t>
+          <t>50006662</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>SON21006021</t>
+          <t>SON21006253</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3450,15 +3450,15 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>30002736</t>
+          <t>30002057</t>
         </is>
       </c>
       <c r="E92" t="n">
-        <v>9000</v>
+        <v>3888</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G92" t="n">
@@ -3468,12 +3468,12 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>50000605</t>
+          <t>50008083</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>SON21006399</t>
+          <t>SON21006574</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3483,15 +3483,15 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>30002113</t>
+          <t>30002283</t>
         </is>
       </c>
       <c r="E93" t="n">
-        <v>20000</v>
+        <v>3000</v>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G93" t="n">
@@ -3501,12 +3501,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>50000609</t>
+          <t>50000314</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>SON21006399</t>
+          <t>SON21007046</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -3516,15 +3516,15 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>30002109</t>
+          <t>30002138</t>
         </is>
       </c>
       <c r="E94" t="n">
-        <v>16000</v>
+        <v>5000</v>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G94" t="n">
@@ -3534,12 +3534,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>50000611</t>
+          <t>50000335</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>SON21006399</t>
+          <t>SON21007046</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3549,15 +3549,15 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>30002108</t>
+          <t>30002141</t>
         </is>
       </c>
       <c r="E95" t="n">
-        <v>16000</v>
+        <v>1600</v>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G95" t="n">
@@ -3567,12 +3567,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>50006679</t>
+          <t>50004282</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>SON21006253</t>
+          <t>SON21007336</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3582,15 +3582,15 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>30002056</t>
+          <t>30002452</t>
         </is>
       </c>
       <c r="E96" t="n">
-        <v>6369</v>
+        <v>25008</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G96" t="n">
@@ -3600,12 +3600,12 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>50006680</t>
+          <t>50000483</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>SON21006253</t>
+          <t>SON21007888</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3615,15 +3615,15 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>30002056</t>
+          <t>30002094</t>
         </is>
       </c>
       <c r="E97" t="n">
-        <v>2926</v>
+        <v>53760</v>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G97" t="n">
@@ -3633,12 +3633,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>50006661</t>
+          <t>50000483</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>SON21006253</t>
+          <t>SON21008029</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3648,15 +3648,15 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>30002057</t>
+          <t>30002094</t>
         </is>
       </c>
       <c r="E98" t="n">
-        <v>4950</v>
+        <v>82560</v>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G98" t="n">
@@ -3666,12 +3666,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>50006662</t>
+          <t>50008144</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>SON21006253</t>
+          <t>SON21008157</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3681,15 +3681,15 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>30002057</t>
+          <t>30003976</t>
         </is>
       </c>
       <c r="E99" t="n">
-        <v>3888</v>
+        <v>4180</v>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G99" t="n">
@@ -3699,12 +3699,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>50008083</t>
+          <t>50000552</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>SON21006574</t>
+          <t>SON21008295</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3714,15 +3714,15 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>30002283</t>
+          <t>30002471</t>
         </is>
       </c>
       <c r="E100" t="n">
-        <v>3000</v>
+        <v>10483</v>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G100" t="n">
@@ -3732,12 +3732,12 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>50000314</t>
+          <t>50008144</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>SON21007046</t>
+          <t>SON21005185</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3747,15 +3747,15 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>30002138</t>
+          <t>30003976</t>
         </is>
       </c>
       <c r="E101" t="n">
-        <v>5000</v>
+        <v>3630</v>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G101" t="n">
@@ -3765,12 +3765,12 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>50000335</t>
+          <t>50008760</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>SON21007046</t>
+          <t>SON21008753</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3780,15 +3780,15 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>30002141</t>
+          <t>30002736</t>
         </is>
       </c>
       <c r="E102" t="n">
-        <v>1600</v>
+        <v>9000</v>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G102" t="n">
@@ -3798,12 +3798,12 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>50004282</t>
+          <t>50006001</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>SON21007336</t>
+          <t>SON21008837</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3813,15 +3813,15 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>30002452</t>
+          <t>30002063</t>
         </is>
       </c>
       <c r="E103" t="n">
-        <v>25008</v>
+        <v>6000</v>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G103" t="n">
@@ -3831,12 +3831,12 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>50000483</t>
+          <t>50004282</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>SON21007888</t>
+          <t>SON21008756</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3846,15 +3846,15 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>30002094</t>
+          <t>30002452</t>
         </is>
       </c>
       <c r="E104" t="n">
-        <v>53760</v>
+        <v>25008</v>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G104" t="n">
@@ -3864,12 +3864,12 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>50000483</t>
+          <t>50008064</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>SON21008029</t>
+          <t>SON21008812</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3879,15 +3879,15 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>30002094</t>
+          <t>30002018</t>
         </is>
       </c>
       <c r="E105" t="n">
-        <v>82560</v>
+        <v>20635</v>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G105" t="n">
@@ -3897,12 +3897,12 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>50008144</t>
+          <t>50005991</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>SON21008157</t>
+          <t>SON21008765</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3912,15 +3912,15 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>30003976</t>
+          <t>30002061</t>
         </is>
       </c>
       <c r="E106" t="n">
-        <v>4180</v>
+        <v>6000</v>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G106" t="n">
@@ -3930,30 +3930,30 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>50000552</t>
+          <t>50006621</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>SON21008295</t>
+          <t>SON21002400</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>At least one component has no extrusion rate</t>
+          <t>Finished good has no packing rate</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>30002471</t>
+          <t>30000115</t>
         </is>
       </c>
       <c r="E107" t="n">
-        <v>10483</v>
+        <v>1664</v>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G107" t="n">
@@ -3963,30 +3963,30 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>50008144</t>
+          <t>50000792</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>SON21005185</t>
+          <t>SON21006639</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>At least one component has no extrusion rate</t>
+          <t>Finished good has no packing rate</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>30003976</t>
+          <t>30000363</t>
         </is>
       </c>
       <c r="E108" t="n">
-        <v>3630</v>
+        <v>47616</v>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G108" t="n">
@@ -3996,12 +3996,12 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>50006621</t>
+          <t>50000803</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>SON21002400</t>
+          <t>SON21006639</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -4011,15 +4011,15 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>30000115</t>
+          <t>30000361</t>
         </is>
       </c>
       <c r="E109" t="n">
-        <v>1664</v>
+        <v>222250</v>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G109" t="n">
@@ -4029,7 +4029,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>50000792</t>
+          <t>50000796</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -4044,15 +4044,15 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>30000363</t>
+          <t>30000361</t>
         </is>
       </c>
       <c r="E110" t="n">
-        <v>47616</v>
+        <v>10800</v>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G110" t="n">
@@ -4062,7 +4062,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>50000803</t>
+          <t>50000800</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -4077,15 +4077,15 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>30000361</t>
+          <t>30000377</t>
         </is>
       </c>
       <c r="E111" t="n">
-        <v>222250</v>
+        <v>143904</v>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G111" t="n">
@@ -4095,7 +4095,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>50000796</t>
+          <t>50000793</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -4110,15 +4110,15 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>30000361</t>
+          <t>30000377</t>
         </is>
       </c>
       <c r="E112" t="n">
-        <v>10800</v>
+        <v>29592</v>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G112" t="n">
@@ -4128,7 +4128,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>50000800</t>
+          <t>50000797</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -4143,15 +4143,15 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>30000377</t>
+          <t>30000360</t>
         </is>
       </c>
       <c r="E113" t="n">
-        <v>143904</v>
+        <v>24792</v>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G113" t="n">
@@ -4161,7 +4161,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>50000793</t>
+          <t>50009180</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -4176,15 +4176,15 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>30000377</t>
+          <t>30000360</t>
         </is>
       </c>
       <c r="E114" t="n">
-        <v>29592</v>
+        <v>115962</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G114" t="n">
@@ -4194,7 +4194,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>50000797</t>
+          <t>50000794</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -4213,11 +4213,11 @@
         </is>
       </c>
       <c r="E115" t="n">
-        <v>24792</v>
+        <v>80496</v>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G115" t="n">
@@ -4227,7 +4227,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>50009180</t>
+          <t>50000799</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -4242,15 +4242,15 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>30000360</t>
+          <t>30000361</t>
         </is>
       </c>
       <c r="E116" t="n">
-        <v>115962</v>
+        <v>7248</v>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G116" t="n">
@@ -4260,12 +4260,12 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>50000794</t>
+          <t>50006671</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>SON21006639</t>
+          <t>SON21002773</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -4275,15 +4275,15 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>30000360</t>
+          <t>30000114</t>
         </is>
       </c>
       <c r="E117" t="n">
-        <v>80496</v>
+        <v>5500</v>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G117" t="n">
@@ -4293,12 +4293,12 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>50000799</t>
+          <t>50006622</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>SON21006639</t>
+          <t>SON21002773</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -4308,15 +4308,15 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>30000361</t>
+          <t>30000114</t>
         </is>
       </c>
       <c r="E118" t="n">
-        <v>7248</v>
+        <v>10920</v>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G118" t="n">
@@ -4326,12 +4326,12 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>50006671</t>
+          <t>50000647</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>SON21002773</t>
+          <t>SON21002400</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -4341,15 +4341,15 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>30000114</t>
+          <t>30000521</t>
         </is>
       </c>
       <c r="E119" t="n">
-        <v>5500</v>
+        <v>16500</v>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G119" t="n">
@@ -4359,12 +4359,12 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>50006622</t>
+          <t>50000659</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>SON21002773</t>
+          <t>SON21002400</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -4374,15 +4374,15 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>30000114</t>
+          <t>30000523</t>
         </is>
       </c>
       <c r="E120" t="n">
-        <v>10920</v>
+        <v>5712</v>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G120" t="n">
@@ -4392,7 +4392,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>50000647</t>
+          <t>50006671</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -4407,15 +4407,15 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>30000521</t>
+          <t>30000114</t>
         </is>
       </c>
       <c r="E121" t="n">
-        <v>16500</v>
+        <v>660</v>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G121" t="n">
@@ -4425,7 +4425,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>50000659</t>
+          <t>50006622</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -4440,15 +4440,15 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>30000523</t>
+          <t>30000114</t>
         </is>
       </c>
       <c r="E122" t="n">
-        <v>5712</v>
+        <v>11050</v>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G122" t="n">
@@ -4458,7 +4458,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>50006671</t>
+          <t>50006623</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -4473,15 +4473,15 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>30000114</t>
+          <t>30000116</t>
         </is>
       </c>
       <c r="E123" t="n">
-        <v>660</v>
+        <v>1079</v>
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G123" t="n">
@@ -4491,7 +4491,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>50006622</t>
+          <t>50006669</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -4506,15 +4506,15 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>30000114</t>
+          <t>30000115</t>
         </is>
       </c>
       <c r="E124" t="n">
-        <v>11050</v>
+        <v>1870</v>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G124" t="n">
@@ -4524,12 +4524,12 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>50006623</t>
+          <t>50000647</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>SON21002400</t>
+          <t>SON21002773</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -4539,15 +4539,15 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>30000116</t>
+          <t>30000521</t>
         </is>
       </c>
       <c r="E125" t="n">
-        <v>1079</v>
+        <v>6050</v>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G125" t="n">
@@ -4557,12 +4557,12 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>50006669</t>
+          <t>50000401</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>SON21002400</t>
+          <t>SON21006148</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -4572,15 +4572,15 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>30000115</t>
+          <t>30000729</t>
         </is>
       </c>
       <c r="E126" t="n">
-        <v>1870</v>
+        <v>200004</v>
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G126" t="n">
@@ -4590,12 +4590,12 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>50000647</t>
+          <t>50000410</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>SON21002773</t>
+          <t>SON21006148</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -4605,15 +4605,15 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>30000521</t>
+          <t>30000732</t>
         </is>
       </c>
       <c r="E127" t="n">
-        <v>6050</v>
+        <v>1998</v>
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G127" t="n">
@@ -4623,7 +4623,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>50000401</t>
+          <t>50000411</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -4638,15 +4638,15 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>30000729</t>
+          <t>30000732</t>
         </is>
       </c>
       <c r="E128" t="n">
-        <v>200004</v>
+        <v>12002</v>
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G128" t="n">
@@ -4656,7 +4656,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>50000410</t>
+          <t>50000412</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -4675,11 +4675,11 @@
         </is>
       </c>
       <c r="E129" t="n">
-        <v>1998</v>
+        <v>186004</v>
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G129" t="n">
@@ -4689,7 +4689,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>50000411</t>
+          <t>50000413</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -4704,15 +4704,15 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>30000732</t>
+          <t>30000734</t>
         </is>
       </c>
       <c r="E130" t="n">
-        <v>12002</v>
+        <v>15012</v>
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G130" t="n">
@@ -4722,7 +4722,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>50000412</t>
+          <t>50000414</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -4737,15 +4737,15 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>30000732</t>
+          <t>30000734</t>
         </is>
       </c>
       <c r="E131" t="n">
-        <v>186004</v>
+        <v>44996</v>
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G131" t="n">
@@ -4755,7 +4755,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>50000413</t>
+          <t>50000415</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -4774,11 +4774,11 @@
         </is>
       </c>
       <c r="E132" t="n">
-        <v>15012</v>
+        <v>140000</v>
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G132" t="n">
@@ -4788,12 +4788,12 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>50000414</t>
+          <t>50000401</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>SON21006148</t>
+          <t>SON21006849</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -4803,15 +4803,15 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>30000734</t>
+          <t>30000729</t>
         </is>
       </c>
       <c r="E133" t="n">
-        <v>44996</v>
+        <v>200004</v>
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G133" t="n">
@@ -4821,12 +4821,12 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>50000415</t>
+          <t>50000397</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>SON21006148</t>
+          <t>SON21006849</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -4836,15 +4836,15 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>30000734</t>
+          <t>30000728</t>
         </is>
       </c>
       <c r="E134" t="n">
-        <v>140000</v>
+        <v>15012</v>
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G134" t="n">
@@ -4854,7 +4854,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>50000397</t>
+          <t>50000398</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -4873,11 +4873,11 @@
         </is>
       </c>
       <c r="E135" t="n">
-        <v>15012</v>
+        <v>19994</v>
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G135" t="n">
@@ -4887,7 +4887,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>50000398</t>
+          <t>50000399</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -4906,11 +4906,11 @@
         </is>
       </c>
       <c r="E136" t="n">
-        <v>19994</v>
+        <v>365008</v>
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G136" t="n">
@@ -4920,7 +4920,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>50000399</t>
+          <t>50000410</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -4935,15 +4935,15 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>30000728</t>
+          <t>30000732</t>
         </is>
       </c>
       <c r="E137" t="n">
-        <v>365008</v>
+        <v>25002</v>
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G137" t="n">
@@ -4953,12 +4953,12 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>50000649</t>
+          <t>50000411</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>SON21002400</t>
+          <t>SON21006849</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -4968,15 +4968,15 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>30000523</t>
+          <t>30000732</t>
         </is>
       </c>
       <c r="E138" t="n">
-        <v>990</v>
+        <v>14998</v>
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G138" t="n">
@@ -4986,12 +4986,12 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>50006611</t>
+          <t>50000412</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>SON21002400</t>
+          <t>SON21006849</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -5001,15 +5001,15 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>30000114</t>
+          <t>30000732</t>
         </is>
       </c>
       <c r="E139" t="n">
-        <v>39700</v>
+        <v>159992</v>
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G139" t="n">
@@ -5019,12 +5019,12 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>50000717</t>
+          <t>50000649</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>SOE21006832</t>
+          <t>SON21002400</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -5034,15 +5034,15 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>30000544</t>
+          <t>30000523</t>
         </is>
       </c>
       <c r="E140" t="n">
-        <v>1134</v>
+        <v>990</v>
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G140" t="n">
@@ -5052,12 +5052,12 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>50000717</t>
+          <t>50006611</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>SOE21006990</t>
+          <t>SON21002400</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -5067,15 +5067,15 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>30000544</t>
+          <t>30000114</t>
         </is>
       </c>
       <c r="E141" t="n">
-        <v>1134</v>
+        <v>39700</v>
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G141" t="n">
@@ -5090,7 +5090,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>SOE21007472</t>
+          <t>SOE21006832</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -5104,11 +5104,11 @@
         </is>
       </c>
       <c r="E142" t="n">
-        <v>5670</v>
+        <v>1134</v>
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G142" t="n">
@@ -5123,7 +5123,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>SOE21007569</t>
+          <t>SOE21006990</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -5141,7 +5141,7 @@
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G143" t="n">
@@ -5156,7 +5156,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>SOE21007536</t>
+          <t>SOE21007855</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -5174,10 +5174,109 @@
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-10-06</t>
         </is>
       </c>
       <c r="G144" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>50000717</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>SOE21007839</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Finished good has no packing rate</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>30000544</t>
+        </is>
+      </c>
+      <c r="E145" t="n">
+        <v>4536</v>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>2021-10-06</t>
+        </is>
+      </c>
+      <c r="G145" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>50000717</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>SOE21007569</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Finished good has no packing rate</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>30000544</t>
+        </is>
+      </c>
+      <c r="E146" t="n">
+        <v>4536</v>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>2021-10-06</t>
+        </is>
+      </c>
+      <c r="G146" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>50000717</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>SOE21007536</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Finished good has no packing rate</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>30000544</t>
+        </is>
+      </c>
+      <c r="E147" t="n">
+        <v>4536</v>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>2021-10-06</t>
+        </is>
+      </c>
+      <c r="G147" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>